<commit_message>
begun transferring to latex
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connall\Desktop\DISS_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DA8A9E-B7D9-4919-B997-DC8B4630910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B547BF-AFD5-4F89-B126-BEF784E60E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2835" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -50,54 +50,21 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Literature Review</t>
-  </si>
-  <si>
     <t>Draft</t>
   </si>
   <si>
-    <t>Reorganise automated reconfiguration section</t>
-  </si>
-  <si>
     <t>Add key technologies I will use</t>
   </si>
   <si>
-    <t>Edit gaps and opportunities</t>
-  </si>
-  <si>
     <t>Write Project Scope</t>
   </si>
   <si>
     <t>Write Abstract</t>
   </si>
   <si>
-    <t>Write Acknowledgements</t>
-  </si>
-  <si>
-    <t>Write Software Design - Motion planning section</t>
-  </si>
-  <si>
-    <t>Write implementation - state queue class</t>
-  </si>
-  <si>
     <t>Write implementation - state class</t>
   </si>
   <si>
-    <t>Write implementation - module class</t>
-  </si>
-  <si>
-    <t>Write implementation - motion planning</t>
-  </si>
-  <si>
-    <t>Write implementation - feedback strategy</t>
-  </si>
-  <si>
-    <t>Write testing and results - testing method</t>
-  </si>
-  <si>
-    <t>Write testing and results - performance metric</t>
-  </si>
-  <si>
     <t>Write testing and results - analysis of results</t>
   </si>
   <si>
@@ -110,30 +77,12 @@
     <t>Write discussion - implications</t>
   </si>
   <si>
-    <t>Expand Project Management Procedures section</t>
-  </si>
-  <si>
-    <t>Expand Project Management Reflection section</t>
-  </si>
-  <si>
-    <t>Write Risk assessment</t>
-  </si>
-  <si>
-    <t>Write evolution of project plan section</t>
-  </si>
-  <si>
-    <t>Mention discovered problem in last week to management reflection section</t>
-  </si>
-  <si>
     <t>Write Conclusion</t>
   </si>
   <si>
     <t>Write Further Work section</t>
   </si>
   <si>
-    <t>Convert matrix data structure to dictionary to improve memory</t>
-  </si>
-  <si>
     <t>Waiting on text</t>
   </si>
   <si>
@@ -161,15 +110,6 @@
     <t>Update planner</t>
   </si>
   <si>
-    <t>Create advanced motion planner</t>
-  </si>
-  <si>
-    <t>Create graph trimming function</t>
-  </si>
-  <si>
-    <t>Implement feedback strategies</t>
-  </si>
-  <si>
     <t>Software - Logic</t>
   </si>
   <si>
@@ -185,33 +125,12 @@
     <t>Manipulator base location planning</t>
   </si>
   <si>
-    <t>Make matching modules by ID an option</t>
-  </si>
-  <si>
-    <t>Explain module matching by colour is a replacement for matching by type</t>
-  </si>
-  <si>
     <t>Add arm to reconfiguration video</t>
   </si>
   <si>
-    <t>Create basic motion planner (can only grab from above like in gravity enviro)</t>
-  </si>
-  <si>
-    <t>Add Module connection property (some faces can't connect)</t>
-  </si>
-  <si>
-    <t>Add Module orientation property</t>
-  </si>
-  <si>
-    <t>Create output formatter to create and save list of instructions</t>
-  </si>
-  <si>
     <t>Review Software Design and Development</t>
   </si>
   <si>
-    <t>Compare state to goal on generation, not when reached by search</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -264,13 +183,16 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Expand project Objectives and Specifications to include requirements for each goal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,13 +204,6 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,11 +254,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -405,14 +315,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -421,25 +330,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="4"/>
-    <xf numFmtId="10" fontId="4" fillId="7" borderId="3" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3"/>
+    <xf numFmtId="10" fontId="3" fillId="6" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="4" builtinId="21"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
+          <fgColor rgb="FFF8696B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -447,7 +354,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
+          <fgColor rgb="FFF8696B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -455,7 +362,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
+          <fgColor rgb="FFF8696B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -463,63 +370,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
+          <fgColor rgb="FFF8696B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -816,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N59"/>
+  <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,52 +681,53 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="10">
+        <v>3</v>
+      </c>
+      <c r="G2" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Draft*")</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H2" s="7">
         <f>G2/$G$5</f>
-        <v>0.58139534883720934</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="10">
+        <v>42</v>
+      </c>
+      <c r="G3" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Software*")</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" ref="H3:H4" si="0">G3/$G$5</f>
-        <v>0.34883720930232559</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="N3">
         <v>10</v>
@@ -883,27 +735,27 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="10">
+        <v>43</v>
+      </c>
+      <c r="G4" s="9">
         <f>COUNTIF(C$12:C$1048576,"*") - G3 - G2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="0"/>
-        <v>6.9767441860465115E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="N4">
         <v>10</v>
@@ -911,23 +763,23 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="11">
+        <v>44</v>
+      </c>
+      <c r="G5" s="6">
         <f>SUM(G2:G4)</f>
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="N5">
         <v>5</v>
@@ -935,16 +787,16 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F6" s="8" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="G6" s="6">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="N6">
         <v>15</v>
@@ -952,29 +804,29 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L9" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -993,22 +845,21 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="9"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -1016,10 +867,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -1027,21 +878,24 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -1049,32 +903,32 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -1082,21 +936,21 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -1104,37 +958,37 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1145,24 +999,24 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -1170,309 +1024,34 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="4">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="4">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="4">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4">
-        <v>0</v>
-      </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4">
-        <v>0</v>
-      </c>
-      <c r="C49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4">
-        <v>0</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
-        <v>0</v>
-      </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4">
-        <v>0</v>
-      </c>
-      <c r="C52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4">
-        <v>0</v>
-      </c>
-      <c r="C53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="B30" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B11:D54" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D54">
-      <sortCondition sortBy="cellColor" ref="D11:D54" dxfId="1"/>
+  <autoFilter ref="B11:D26" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D28">
+      <sortCondition sortBy="cellColor" ref="B11:B26" dxfId="3"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="B12:B54 B59">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B12:B30">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Moving draft to latex
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connall\Desktop\DISS_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B547BF-AFD5-4F89-B126-BEF784E60E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7652A375-86FE-4B8E-9AE1-2D361740B316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2835" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -56,33 +56,9 @@
     <t>Add key technologies I will use</t>
   </si>
   <si>
-    <t>Write Project Scope</t>
-  </si>
-  <si>
     <t>Write Abstract</t>
   </si>
   <si>
-    <t>Write implementation - state class</t>
-  </si>
-  <si>
-    <t>Write testing and results - analysis of results</t>
-  </si>
-  <si>
-    <t>Write discussion - interpretation of results</t>
-  </si>
-  <si>
-    <t>Write discussion - comparison to existing work</t>
-  </si>
-  <si>
-    <t>Write discussion - implications</t>
-  </si>
-  <si>
-    <t>Write Conclusion</t>
-  </si>
-  <si>
-    <t>Write Further Work section</t>
-  </si>
-  <si>
     <t>Waiting on text</t>
   </si>
   <si>
@@ -122,15 +98,6 @@
     <t>Software - Main</t>
   </si>
   <si>
-    <t>Manipulator base location planning</t>
-  </si>
-  <si>
-    <t>Add arm to reconfiguration video</t>
-  </si>
-  <si>
-    <t>Review Software Design and Development</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -182,10 +149,13 @@
     <t>REMINDER: You are handing in a dissertation, not code. Talking about your resultant code is more important that having resultant code (they'll not read it)</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Expand project Objectives and Specifications to include requirements for each goal</t>
+  </si>
+  <si>
+    <t>Add code to latex</t>
+  </si>
+  <si>
+    <t>Format Pseudo-code figures</t>
   </si>
 </sst>
 </file>
@@ -321,7 +291,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -334,7 +304,6 @@
     <xf numFmtId="10" fontId="3" fillId="6" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -342,51 +311,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8696B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8696B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8696B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8696B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -667,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N30"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,46 +617,46 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Draft*")</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H2" s="7">
         <f>G2/$G$5</f>
-        <v>0.66666666666666663</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G3" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Software*")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" ref="H3:H4" si="0">G3/$G$5</f>
-        <v>0.27777777777777779</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <v>10</v>
@@ -735,13 +664,13 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G4" s="9">
         <f>COUNTIF(C$12:C$1048576,"*") - G3 - G2</f>
@@ -749,13 +678,13 @@
       </c>
       <c r="H4" s="7">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N4">
         <v>10</v>
@@ -763,40 +692,34 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G5" s="6">
         <f>SUM(G2:G4)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N5">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="6">
-        <v>26</v>
-      </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="N6">
         <v>15</v>
@@ -804,29 +727,29 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -847,77 +770,74 @@
       <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -927,131 +847,29 @@
       <c r="C19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
+      <c r="D19" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B11:D26" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D28">
-      <sortCondition sortBy="cellColor" ref="B11:B26" dxfId="3"/>
+  <autoFilter ref="B11:D16" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D18">
+      <sortCondition sortBy="cellColor" ref="B11:B16" dxfId="0"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="B12:B30">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="B12:B20">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
First Latex draft without code done
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connall\Desktop\DISS_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A2342B-EB14-4E96-A26E-C4B4C630DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FFC88A-A30B-4C94-AFDB-FAE9C9E17187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2835" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$11:$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -77,9 +77,6 @@
     <t>3 - little effect but nice to have</t>
   </si>
   <si>
-    <t>Project Planner</t>
-  </si>
-  <si>
     <t>Software - Logic</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>REMINDER: You are handing in a dissertation, not code. Talking about your resultant code is more important that having resultant code (they'll not read it)</t>
   </si>
   <si>
-    <t>Expand project Objectives and Specifications to include requirements for each goal</t>
-  </si>
-  <si>
     <t>Add code to latex</t>
   </si>
   <si>
@@ -155,7 +149,22 @@
     <t>Add listings / Figures list</t>
   </si>
   <si>
-    <t>Update planner and add to draft</t>
+    <t>Review Project Management section</t>
+  </si>
+  <si>
+    <t>Correct references from feedback</t>
+  </si>
+  <si>
+    <t>Saturday:</t>
+  </si>
+  <si>
+    <t>Sunday:</t>
+  </si>
+  <si>
+    <t>Final Edit</t>
+  </si>
+  <si>
+    <t>Format Code</t>
   </si>
 </sst>
 </file>
@@ -604,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N20"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,14 +641,14 @@
       </c>
       <c r="G2" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Draft*")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="7">
         <f>G2/$G$5</f>
-        <v>0.55555555555555558</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -650,7 +659,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="9">
         <f>COUNTIF(C$12:C$1048576,"*Software*")</f>
@@ -661,10 +670,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N3">
         <v>10</v>
@@ -678,21 +687,21 @@
         <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="9">
         <f>COUNTIF(C$12:C$1048576,"*") - G3 - G2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N4">
         <v>10</v>
@@ -706,17 +715,17 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="6">
         <f>SUM(G2:G4)</f>
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N5">
         <v>5</v>
@@ -724,10 +733,10 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N6">
         <v>15</v>
@@ -735,29 +744,29 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
         <v>21</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
         <v>25</v>
-      </c>
-      <c r="M8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
         <v>23</v>
-      </c>
-      <c r="M9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -773,24 +782,24 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -798,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -809,10 +818,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -820,35 +829,35 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -859,25 +868,41 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B11:D15" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D17">
-      <sortCondition sortBy="cellColor" ref="B11:B15" dxfId="1"/>
+  <autoFilter ref="B11:D14" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:D20">
+      <sortCondition ref="B11:B14"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>